<commit_message>
Update IP - EX 19 - Funcao Cont.se e Cont.ses (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 19 - Funcao Cont.se e Cont.ses (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 19 - Funcao Cont.se e Cont.ses (Anexo).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172FD11A-1934-4448-B7AF-6743214DB081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D739BFE8-74D7-45C4-A794-C94B6C0C71C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
     <sheet name="EXPLICAÇÃO" sheetId="10" r:id="rId2"/>
-    <sheet name="EXERCICIO 1" sheetId="15" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="16" r:id="rId3"/>
+    <sheet name="EXERCICIO 1" sheetId="15" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="anscount" hidden="1">2</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="50">
   <si>
     <t>NOMES</t>
   </si>
@@ -207,6 +208,9 @@
   </si>
   <si>
     <t>Funções CONTSE e CONTSES</t>
+  </si>
+  <si>
+    <t>FUNÇÃO CONTSES</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1091,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1374,6 +1378,15 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="25" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2097,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,7 +2227,9 @@
       <c r="E8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="68"/>
+      <c r="F8" s="68" t="s">
+        <v>2</v>
+      </c>
       <c r="G8" s="69"/>
       <c r="H8" s="70"/>
     </row>
@@ -2231,9 +2246,12 @@
       <c r="E10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
+      <c r="F10" s="109">
+        <f>COUNTIF($B$11:$B$40,F8)</f>
+        <v>6</v>
+      </c>
+      <c r="G10" s="110"/>
+      <c r="H10" s="111"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
@@ -2500,7 +2518,7 @@
     </row>
     <row r="46" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G46" s="22" t="s">
         <v>37</v>
@@ -3063,10 +3081,91 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D235C6E9-4084-432F-AEBE-280E2CE9FB00}">
+          <x14:formula1>
+            <xm:f>Planilha1!$A$2:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>F8:H8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0C86ED-B037-492F-AEF8-7B5D186CA2A5}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:P502"/>
   <sheetViews>

</xml_diff>